<commit_message>
Grade Update - Started HW 5
began homework 5 - planning
</commit_message>
<xml_diff>
--- a/CSCE 420 Grades.xlsx
+++ b/CSCE 420 Grades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xhunt\Documents\GitHub\TAMU-CSCE-420\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter\Documents\GitHub\TAMU-CSCE-420\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DA9B13-ABFD-4468-8067-DBAB5CCD5425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085CDED8-9704-495F-BB78-A96E59677BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31605" yWindow="2565" windowWidth="13500" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Grading</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ending Grading Estimate= </t>
+  </si>
+  <si>
+    <t>need a 67 on the final</t>
+  </si>
+  <si>
+    <t>need a 73 on programming assignment #5</t>
   </si>
 </sst>
 </file>
@@ -372,25 +378,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E17"/>
+  <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.265625" customWidth="1"/>
+    <col min="4" max="4" width="25.265625" customWidth="1"/>
+    <col min="5" max="5" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -404,7 +410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>0.4</v>
       </c>
@@ -418,12 +424,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1</v>
       </c>
@@ -442,16 +448,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2</v>
       </c>
+      <c r="B8">
+        <f>33/50</f>
+        <v>0.66</v>
+      </c>
       <c r="C8">
         <f>25/25</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3</v>
       </c>
@@ -459,8 +472,11 @@
         <f>10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>4</v>
       </c>
@@ -468,18 +484,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14">
         <f>AVERAGE(B7:B11)</f>
-        <v>0.77966101694915257</v>
+        <v>0.7198305084745763</v>
       </c>
       <c r="C14">
         <f>AVERAGE(C7:C11)</f>
@@ -494,13 +510,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17">
         <f>B14*B4+C14*C4+D14*D4+E14*E4</f>
-        <v>0.830864406779661</v>
+        <v>0.80693220338983063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>